<commit_message>
T4.1 update data extraction files and bycatch case study
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Dinesen.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Dinesen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/estb_dtu_dk/Documents/Projects/SEAwise/T4.1/Data extraction/Read only SP files to be uploaded_SP issues Nov22/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="13_ncr:1_{2280A903-DAC0-4C4B-8BBE-75D81ED3D1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1DFE284-BEC5-45D4-90D3-D1735E4FA70D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC264080-14EB-436A-847C-94967F60878D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4650" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$44</definedName>
     <definedName name="Benthic_epifauna">Validation!$AI$32:$AI$35</definedName>
     <definedName name="Benthos">Validation!$AN$24:$AN$25</definedName>
     <definedName name="Catch_and_bycatch">Validation!$AM$15:$AM$17</definedName>
@@ -2392,7 +2392,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="368">
   <si>
     <t>SearchID</t>
   </si>
@@ -3495,6 +3495,9 @@
   <si>
     <t>Closing all the study area to fishing activities (scenario 4) would bring common dolphins by 2030 to biomass levels similar to those observed in 2004 (approximately 50 individuals) while sardines and anchovies would keep the same
 trajectories as delineated in the previous scenario.</t>
+  </si>
+  <si>
+    <t>bycatch was unlikely to be the main cause of the decline</t>
   </si>
 </sst>
 </file>
@@ -3633,7 +3636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3647,13 +3650,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3676,7 +3677,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3700,7 +3700,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Validation"/>
@@ -3710,10 +3710,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3979,12 +3975,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX43"/>
+  <dimension ref="A1:AX44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="AP17" sqref="AP17"/>
+      <selection pane="bottomLeft" activeCell="AX11" sqref="AX11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4006,70 +4002,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="18" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="16" t="s">
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="17" t="s">
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="17"/>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="17"/>
-      <c r="AM1" s="19" t="s">
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="13" t="s">
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="14" t="s">
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AV1" s="14"/>
-      <c r="AW1" s="14"/>
-      <c r="AX1" s="14"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
     </row>
     <row r="2" spans="1:50" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -4224,7 +4220,7 @@
       </c>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" t="s">
         <v>305</v>
       </c>
       <c r="B3" t="s">
@@ -4346,7 +4342,7 @@
       </c>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" t="s">
         <v>305</v>
       </c>
       <c r="B4" t="s">
@@ -4468,7 +4464,7 @@
       </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="A5" t="s">
         <v>305</v>
       </c>
       <c r="B5" t="s">
@@ -4590,7 +4586,7 @@
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" t="s">
         <v>305</v>
       </c>
       <c r="B6" t="s">
@@ -4712,7 +4708,7 @@
       </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="A7" t="s">
         <v>300</v>
       </c>
       <c r="B7" t="s">
@@ -4796,7 +4792,7 @@
       <c r="AE7" t="s">
         <v>329</v>
       </c>
-      <c r="AF7" s="12">
+      <c r="AF7" s="10">
         <v>4.4000000000000004</v>
       </c>
       <c r="AG7" t="s">
@@ -4840,7 +4836,7 @@
       </c>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" t="s">
         <v>300</v>
       </c>
       <c r="B8" t="s">
@@ -4924,7 +4920,7 @@
       <c r="AE8" t="s">
         <v>329</v>
       </c>
-      <c r="AF8" s="12">
+      <c r="AF8" s="10">
         <v>4.4000000000000004</v>
       </c>
       <c r="AG8" t="s">
@@ -4968,7 +4964,7 @@
       </c>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="A9" t="s">
         <v>300</v>
       </c>
       <c r="B9" t="s">
@@ -5052,7 +5048,7 @@
       <c r="AE9" t="s">
         <v>329</v>
       </c>
-      <c r="AF9" s="12">
+      <c r="AF9" s="10">
         <v>4.4000000000000004</v>
       </c>
       <c r="AG9" t="s">
@@ -5096,7 +5092,7 @@
       </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" t="s">
         <v>294</v>
       </c>
       <c r="B10" t="s">
@@ -5214,14 +5210,14 @@
         <v>199</v>
       </c>
       <c r="AW10" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="AX10" t="s">
-        <v>352</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="A11" t="s">
         <v>294</v>
       </c>
       <c r="B11" t="s">
@@ -5306,14 +5302,26 @@
         <v>111</v>
       </c>
       <c r="AH11" t="s">
-        <v>117</v>
+        <v>115</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>155</v>
       </c>
       <c r="AK11" t="s">
         <v>150</v>
       </c>
+      <c r="AL11" t="s">
+        <v>331</v>
+      </c>
       <c r="AM11" t="s">
         <v>232</v>
       </c>
+      <c r="AN11" t="s">
+        <v>161</v>
+      </c>
       <c r="AO11" t="s">
         <v>351</v>
       </c>
@@ -5334,7 +5342,7 @@
       </c>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+      <c r="A12" t="s">
         <v>294</v>
       </c>
       <c r="B12" t="s">
@@ -5419,14 +5427,11 @@
         <v>111</v>
       </c>
       <c r="AH12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="AK12" t="s">
         <v>150</v>
       </c>
-      <c r="AL12" t="s">
-        <v>353</v>
-      </c>
       <c r="AM12" t="s">
         <v>232</v>
       </c>
@@ -5437,7 +5442,7 @@
         <v>164</v>
       </c>
       <c r="AU12" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="AV12" t="s">
         <v>199</v>
@@ -5450,7 +5455,7 @@
       </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="A13" t="s">
         <v>294</v>
       </c>
       <c r="B13" t="s">
@@ -5541,7 +5546,7 @@
         <v>150</v>
       </c>
       <c r="AL13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AM13" t="s">
         <v>232</v>
@@ -5553,10 +5558,10 @@
         <v>164</v>
       </c>
       <c r="AU13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AV13" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="AW13" t="s">
         <v>208</v>
@@ -5566,7 +5571,7 @@
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+      <c r="A14" t="s">
         <v>294</v>
       </c>
       <c r="B14" t="s">
@@ -5651,11 +5656,14 @@
         <v>111</v>
       </c>
       <c r="AH14" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="AK14" t="s">
         <v>150</v>
       </c>
+      <c r="AL14" t="s">
+        <v>354</v>
+      </c>
       <c r="AM14" t="s">
         <v>232</v>
       </c>
@@ -5666,20 +5674,20 @@
         <v>164</v>
       </c>
       <c r="AU14" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
       <c r="AV14" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="AW14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AX14" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="A15" t="s">
         <v>294</v>
       </c>
       <c r="B15" t="s">
@@ -5764,53 +5772,35 @@
         <v>111</v>
       </c>
       <c r="AH15" t="s">
-        <v>115</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>129</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="AK15" t="s">
         <v>150</v>
       </c>
-      <c r="AL15" t="s">
-        <v>331</v>
-      </c>
       <c r="AM15" t="s">
         <v>232</v>
       </c>
-      <c r="AN15" t="s">
-        <v>162</v>
-      </c>
       <c r="AO15" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="AQ15" t="s">
         <v>164</v>
       </c>
-      <c r="AR15" t="s">
-        <v>169</v>
-      </c>
-      <c r="AS15" t="s">
-        <v>181</v>
-      </c>
       <c r="AU15" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="AV15" t="s">
         <v>199</v>
       </c>
       <c r="AW15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AX15" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="A16" t="s">
         <v>294</v>
       </c>
       <c r="B16" t="s">
@@ -5913,7 +5903,7 @@
         <v>232</v>
       </c>
       <c r="AN16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AO16" t="s">
         <v>360</v>
@@ -5922,10 +5912,10 @@
         <v>164</v>
       </c>
       <c r="AR16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AS16" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="AU16" t="s">
         <v>358</v>
@@ -5941,7 +5931,7 @@
       </c>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="A17" t="s">
         <v>294</v>
       </c>
       <c r="B17" t="s">
@@ -6044,7 +6034,7 @@
         <v>232</v>
       </c>
       <c r="AN17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AO17" t="s">
         <v>360</v>
@@ -6053,10 +6043,10 @@
         <v>164</v>
       </c>
       <c r="AR17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AS17" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="AU17" t="s">
         <v>358</v>
@@ -6072,7 +6062,7 @@
       </c>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="A18" t="s">
         <v>294</v>
       </c>
       <c r="B18" t="s">
@@ -6157,22 +6147,25 @@
         <v>111</v>
       </c>
       <c r="AH18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AI18" t="s">
-        <v>147</v>
+        <v>129</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>155</v>
       </c>
       <c r="AK18" t="s">
         <v>150</v>
       </c>
       <c r="AL18" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AM18" t="s">
         <v>232</v>
       </c>
       <c r="AN18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AO18" t="s">
         <v>360</v>
@@ -6184,7 +6177,7 @@
         <v>169</v>
       </c>
       <c r="AS18" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="AU18" t="s">
         <v>358</v>
@@ -6195,12 +6188,12 @@
       <c r="AW18" t="s">
         <v>208</v>
       </c>
-      <c r="AX18" s="20" t="s">
-        <v>361</v>
+      <c r="AX18" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="A19" t="s">
         <v>294</v>
       </c>
       <c r="B19" t="s">
@@ -6309,10 +6302,10 @@
         <v>164</v>
       </c>
       <c r="AR19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AS19" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="AU19" t="s">
         <v>358</v>
@@ -6323,12 +6316,12 @@
       <c r="AW19" t="s">
         <v>208</v>
       </c>
-      <c r="AX19" s="20" t="s">
+      <c r="AX19" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+      <c r="A20" t="s">
         <v>294</v>
       </c>
       <c r="B20" t="s">
@@ -6413,53 +6406,50 @@
         <v>111</v>
       </c>
       <c r="AH20" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AI20" t="s">
-        <v>129</v>
-      </c>
-      <c r="AJ20" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="AK20" t="s">
         <v>150</v>
       </c>
       <c r="AL20" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="AM20" t="s">
         <v>232</v>
       </c>
       <c r="AN20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AO20" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="AQ20" t="s">
         <v>164</v>
       </c>
       <c r="AR20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AS20" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="AU20" t="s">
-        <v>343</v>
+        <v>358</v>
       </c>
       <c r="AV20" t="s">
         <v>199</v>
       </c>
       <c r="AW20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AX20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+      <c r="A21" t="s">
         <v>294</v>
       </c>
       <c r="B21" t="s">
@@ -6544,22 +6534,25 @@
         <v>111</v>
       </c>
       <c r="AH21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AI21" t="s">
-        <v>147</v>
+        <v>129</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>155</v>
       </c>
       <c r="AK21" t="s">
         <v>150</v>
       </c>
       <c r="AL21" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AM21" t="s">
         <v>232</v>
       </c>
       <c r="AN21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AO21" t="s">
         <v>357</v>
@@ -6587,7 +6580,7 @@
       </c>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="A22" t="s">
         <v>294</v>
       </c>
       <c r="B22" t="s">
@@ -6672,28 +6665,25 @@
         <v>111</v>
       </c>
       <c r="AH22" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AI22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AJ22" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="AK22" t="s">
         <v>150</v>
       </c>
       <c r="AL22" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="AM22" t="s">
         <v>232</v>
       </c>
       <c r="AN22" t="s">
-        <v>162</v>
-      </c>
-      <c r="AO22" s="20" t="s">
-        <v>364</v>
+        <v>160</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>357</v>
       </c>
       <c r="AQ22" t="s">
         <v>164</v>
@@ -6714,11 +6704,11 @@
         <v>207</v>
       </c>
       <c r="AX22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+      <c r="A23" t="s">
         <v>294</v>
       </c>
       <c r="B23" t="s">
@@ -6821,16 +6811,19 @@
         <v>232</v>
       </c>
       <c r="AN23" t="s">
-        <v>162</v>
-      </c>
-      <c r="AO23" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO23" t="s">
         <v>364</v>
       </c>
       <c r="AQ23" t="s">
         <v>164</v>
       </c>
       <c r="AR23" t="s">
-        <v>239</v>
+        <v>169</v>
+      </c>
+      <c r="AS23" t="s">
+        <v>181</v>
       </c>
       <c r="AU23" t="s">
         <v>343</v>
@@ -6846,7 +6839,7 @@
       </c>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
+      <c r="A24" t="s">
         <v>294</v>
       </c>
       <c r="B24" t="s">
@@ -6949,19 +6942,16 @@
         <v>232</v>
       </c>
       <c r="AN24" t="s">
-        <v>162</v>
-      </c>
-      <c r="AO24" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO24" t="s">
         <v>364</v>
       </c>
       <c r="AQ24" t="s">
         <v>164</v>
       </c>
       <c r="AR24" t="s">
-        <v>169</v>
-      </c>
-      <c r="AS24" t="s">
-        <v>185</v>
+        <v>239</v>
       </c>
       <c r="AU24" t="s">
         <v>343</v>
@@ -6977,7 +6967,7 @@
       </c>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
+      <c r="A25" t="s">
         <v>294</v>
       </c>
       <c r="B25" t="s">
@@ -7080,14 +7070,20 @@
         <v>232</v>
       </c>
       <c r="AN25" t="s">
-        <v>162</v>
-      </c>
-      <c r="AO25" s="20" t="s">
-        <v>365</v>
+        <v>161</v>
+      </c>
+      <c r="AO25" t="s">
+        <v>364</v>
       </c>
       <c r="AQ25" t="s">
         <v>164</v>
       </c>
+      <c r="AR25" t="s">
+        <v>169</v>
+      </c>
+      <c r="AS25" t="s">
+        <v>185</v>
+      </c>
       <c r="AU25" t="s">
         <v>343</v>
       </c>
@@ -7097,12 +7093,12 @@
       <c r="AW25" t="s">
         <v>207</v>
       </c>
-      <c r="AX25" s="20" t="s">
-        <v>366</v>
+      <c r="AX25" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
+      <c r="A26" t="s">
         <v>294</v>
       </c>
       <c r="B26" t="s">
@@ -7187,35 +7183,32 @@
         <v>111</v>
       </c>
       <c r="AH26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AI26" t="s">
-        <v>147</v>
+        <v>129</v>
+      </c>
+      <c r="AJ26" t="s">
+        <v>155</v>
       </c>
       <c r="AK26" t="s">
         <v>150</v>
       </c>
       <c r="AL26" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AM26" t="s">
         <v>232</v>
       </c>
       <c r="AN26" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AO26" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="AQ26" t="s">
         <v>164</v>
       </c>
-      <c r="AR26" t="s">
-        <v>169</v>
-      </c>
-      <c r="AS26" t="s">
-        <v>181</v>
-      </c>
       <c r="AU26" t="s">
         <v>343</v>
       </c>
@@ -7226,11 +7219,11 @@
         <v>207</v>
       </c>
       <c r="AX26" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
+      <c r="A27" t="s">
         <v>294</v>
       </c>
       <c r="B27" t="s">
@@ -7332,8 +7325,8 @@
       <c r="AN27" t="s">
         <v>160</v>
       </c>
-      <c r="AO27" s="20" t="s">
-        <v>364</v>
+      <c r="AO27" t="s">
+        <v>357</v>
       </c>
       <c r="AQ27" t="s">
         <v>164</v>
@@ -7354,11 +7347,11 @@
         <v>207</v>
       </c>
       <c r="AX27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
+      <c r="A28" t="s">
         <v>294</v>
       </c>
       <c r="B28" t="s">
@@ -7460,14 +7453,17 @@
       <c r="AN28" t="s">
         <v>160</v>
       </c>
-      <c r="AO28" s="20" t="s">
+      <c r="AO28" t="s">
         <v>364</v>
       </c>
       <c r="AQ28" t="s">
         <v>164</v>
       </c>
       <c r="AR28" t="s">
-        <v>239</v>
+        <v>169</v>
+      </c>
+      <c r="AS28" t="s">
+        <v>181</v>
       </c>
       <c r="AU28" t="s">
         <v>343</v>
@@ -7483,7 +7479,7 @@
       </c>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A29" s="11" t="s">
+      <c r="A29" t="s">
         <v>294</v>
       </c>
       <c r="B29" t="s">
@@ -7585,17 +7581,14 @@
       <c r="AN29" t="s">
         <v>160</v>
       </c>
-      <c r="AO29" s="20" t="s">
+      <c r="AO29" t="s">
         <v>364</v>
       </c>
       <c r="AQ29" t="s">
         <v>164</v>
       </c>
       <c r="AR29" t="s">
-        <v>169</v>
-      </c>
-      <c r="AS29" t="s">
-        <v>185</v>
+        <v>239</v>
       </c>
       <c r="AU29" t="s">
         <v>343</v>
@@ -7611,7 +7604,7 @@
       </c>
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A30" s="11" t="s">
+      <c r="A30" t="s">
         <v>294</v>
       </c>
       <c r="B30" t="s">
@@ -7713,12 +7706,18 @@
       <c r="AN30" t="s">
         <v>160</v>
       </c>
-      <c r="AO30" s="20" t="s">
-        <v>365</v>
+      <c r="AO30" t="s">
+        <v>364</v>
       </c>
       <c r="AQ30" t="s">
         <v>164</v>
       </c>
+      <c r="AR30" t="s">
+        <v>169</v>
+      </c>
+      <c r="AS30" t="s">
+        <v>185</v>
+      </c>
       <c r="AU30" t="s">
         <v>343</v>
       </c>
@@ -7728,46 +7727,46 @@
       <c r="AW30" t="s">
         <v>207</v>
       </c>
-      <c r="AX30" s="20" t="s">
-        <v>366</v>
+      <c r="AX30" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A31" s="11" t="s">
-        <v>288</v>
+      <c r="A31" t="s">
+        <v>294</v>
       </c>
       <c r="B31" t="s">
         <v>244</v>
       </c>
       <c r="C31" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="D31" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="E31">
         <v>2011</v>
       </c>
       <c r="F31" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="G31">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="H31">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I31">
-        <v>299</v>
+        <v>2490</v>
       </c>
       <c r="J31">
-        <v>316</v>
+        <v>2498</v>
       </c>
       <c r="K31" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="M31" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="N31" t="s">
         <v>243</v>
@@ -7794,10 +7793,13 @@
         <v>55</v>
       </c>
       <c r="X31" t="s">
-        <v>69</v>
+        <v>216</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>330</v>
       </c>
       <c r="Z31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AA31">
         <v>2</v>
@@ -7808,57 +7810,51 @@
       <c r="AC31">
         <v>2</v>
       </c>
-      <c r="AF31">
-        <v>4.2</v>
+      <c r="AF31" t="s">
+        <v>307</v>
       </c>
       <c r="AG31" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AH31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AI31" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="AK31" t="s">
         <v>150</v>
       </c>
       <c r="AL31" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="AM31" t="s">
         <v>232</v>
       </c>
       <c r="AN31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AO31" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="AQ31" t="s">
         <v>164</v>
       </c>
-      <c r="AR31" t="s">
-        <v>197</v>
-      </c>
-      <c r="AS31" t="s">
-        <v>192</v>
-      </c>
       <c r="AU31" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="AV31" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="AW31" t="s">
         <v>207</v>
       </c>
       <c r="AX31" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A32" s="11" t="s">
+      <c r="A32" t="s">
         <v>288</v>
       </c>
       <c r="B32" t="s">
@@ -7964,10 +7960,10 @@
         <v>164</v>
       </c>
       <c r="AR32" t="s">
-        <v>170</v>
+        <v>197</v>
       </c>
       <c r="AS32" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="AU32" t="s">
         <v>347</v>
@@ -7983,7 +7979,7 @@
       </c>
     </row>
     <row r="33" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A33" s="11" t="s">
+      <c r="A33" t="s">
         <v>288</v>
       </c>
       <c r="B33" t="s">
@@ -8089,7 +8085,10 @@
         <v>164</v>
       </c>
       <c r="AR33" t="s">
-        <v>239</v>
+        <v>170</v>
+      </c>
+      <c r="AS33" t="s">
+        <v>190</v>
       </c>
       <c r="AU33" t="s">
         <v>347</v>
@@ -8105,38 +8104,41 @@
       </c>
     </row>
     <row r="34" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A34" s="11" t="s">
-        <v>282</v>
+      <c r="A34" t="s">
+        <v>288</v>
       </c>
       <c r="B34" t="s">
         <v>244</v>
       </c>
       <c r="C34" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D34" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="E34">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="F34" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="G34">
-        <v>414</v>
+        <v>12</v>
+      </c>
+      <c r="H34">
+        <v>3</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>299</v>
       </c>
       <c r="J34">
-        <v>9</v>
+        <v>316</v>
       </c>
       <c r="K34" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="M34" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="N34" t="s">
         <v>243</v>
@@ -8144,14 +8146,11 @@
       <c r="O34" t="s">
         <v>242</v>
       </c>
-      <c r="P34" t="s">
-        <v>245</v>
-      </c>
       <c r="Q34" t="s">
         <v>21</v>
       </c>
       <c r="S34" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="T34" t="s">
         <v>46</v>
@@ -8166,49 +8165,46 @@
         <v>55</v>
       </c>
       <c r="X34" t="s">
-        <v>215</v>
+        <v>69</v>
       </c>
       <c r="Z34" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AA34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB34">
+        <v>1</v>
+      </c>
+      <c r="AC34">
         <v>2</v>
       </c>
-      <c r="AC34">
-        <v>3</v>
-      </c>
-      <c r="AE34" t="s">
-        <v>334</v>
-      </c>
       <c r="AF34">
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="AG34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AH34" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="AI34" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="AK34" t="s">
         <v>150</v>
       </c>
       <c r="AL34" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="AM34" t="s">
         <v>232</v>
       </c>
       <c r="AN34" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AO34" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="AQ34" t="s">
         <v>164</v>
@@ -8216,24 +8212,21 @@
       <c r="AR34" t="s">
         <v>239</v>
       </c>
-      <c r="AS34" t="s">
-        <v>175</v>
-      </c>
       <c r="AU34" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AV34" t="s">
-        <v>205</v>
+        <v>238</v>
       </c>
       <c r="AW34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AX34" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A35" s="11" t="s">
+      <c r="A35" t="s">
         <v>282</v>
       </c>
       <c r="B35" t="s">
@@ -8279,7 +8272,7 @@
         <v>21</v>
       </c>
       <c r="S35" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="T35" t="s">
         <v>46</v>
@@ -8336,7 +8329,7 @@
         <v>160</v>
       </c>
       <c r="AO35" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AQ35" t="s">
         <v>164</v>
@@ -8361,7 +8354,7 @@
       </c>
     </row>
     <row r="36" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A36" s="11" t="s">
+      <c r="A36" t="s">
         <v>282</v>
       </c>
       <c r="B36" t="s">
@@ -8407,7 +8400,7 @@
         <v>21</v>
       </c>
       <c r="S36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T36" t="s">
         <v>46</v>
@@ -8464,7 +8457,7 @@
         <v>160</v>
       </c>
       <c r="AO36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AQ36" t="s">
         <v>164</v>
@@ -8489,41 +8482,38 @@
       </c>
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A37" s="11" t="s">
-        <v>276</v>
+      <c r="A37" t="s">
+        <v>282</v>
       </c>
       <c r="B37" t="s">
         <v>244</v>
       </c>
       <c r="C37" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="D37" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="E37">
         <v>2010</v>
       </c>
       <c r="F37" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="G37">
-        <v>6</v>
-      </c>
-      <c r="H37">
-        <v>2</v>
+        <v>414</v>
       </c>
       <c r="I37">
-        <v>261</v>
+        <v>1</v>
       </c>
       <c r="J37">
-        <v>264</v>
+        <v>9</v>
       </c>
       <c r="K37" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="M37" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="N37" t="s">
         <v>243</v>
@@ -8532,54 +8522,129 @@
         <v>242</v>
       </c>
       <c r="P37" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q37" t="s">
         <v>21</v>
       </c>
-      <c r="R37" t="s">
-        <v>84</v>
+      <c r="S37" t="s">
+        <v>29</v>
+      </c>
+      <c r="T37" t="s">
+        <v>46</v>
+      </c>
+      <c r="U37" t="s">
+        <v>58</v>
+      </c>
+      <c r="V37" t="s">
+        <v>46</v>
+      </c>
+      <c r="W37" t="s">
+        <v>55</v>
+      </c>
+      <c r="X37" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>341</v>
+      </c>
+      <c r="AA37">
+        <v>3</v>
+      </c>
+      <c r="AB37">
+        <v>2</v>
+      </c>
+      <c r="AC37">
+        <v>3</v>
       </c>
       <c r="AE37" t="s">
-        <v>335</v>
-      </c>
-      <c r="AF37" t="s">
-        <v>306</v>
+        <v>334</v>
+      </c>
+      <c r="AF37">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH37" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>317</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN37" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO37" t="s">
+        <v>338</v>
+      </c>
+      <c r="AQ37" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR37" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS37" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU37" t="s">
+        <v>348</v>
+      </c>
+      <c r="AV37" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW37" t="s">
+        <v>210</v>
+      </c>
+      <c r="AX37" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A38" s="11" t="s">
-        <v>270</v>
+      <c r="A38" t="s">
+        <v>276</v>
       </c>
       <c r="B38" t="s">
         <v>244</v>
       </c>
       <c r="C38" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D38" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="E38">
         <v>2010</v>
       </c>
       <c r="F38" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="G38">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38">
-        <v>25</v>
+        <v>261</v>
       </c>
       <c r="J38">
-        <v>30</v>
+        <v>264</v>
+      </c>
+      <c r="K38" t="s">
+        <v>272</v>
       </c>
       <c r="M38" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="N38" t="s">
         <v>243</v>
@@ -8587,6 +8652,9 @@
       <c r="O38" t="s">
         <v>242</v>
       </c>
+      <c r="P38" t="s">
+        <v>247</v>
+      </c>
       <c r="Q38" t="s">
         <v>21</v>
       </c>
@@ -8594,48 +8662,45 @@
         <v>84</v>
       </c>
       <c r="AE38" t="s">
-        <v>349</v>
-      </c>
-      <c r="AF38">
-        <v>4.2</v>
+        <v>335</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A39" s="11" t="s">
-        <v>265</v>
+      <c r="A39" t="s">
+        <v>270</v>
       </c>
       <c r="B39" t="s">
         <v>244</v>
       </c>
       <c r="C39" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D39" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="E39">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="F39" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="G39">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I39">
-        <v>472</v>
+        <v>25</v>
       </c>
       <c r="J39">
-        <v>478</v>
-      </c>
-      <c r="K39" t="s">
-        <v>261</v>
+        <v>30</v>
       </c>
       <c r="M39" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="N39" t="s">
         <v>243</v>
@@ -8646,90 +8711,18 @@
       <c r="Q39" t="s">
         <v>21</v>
       </c>
-      <c r="S39" t="s">
-        <v>31</v>
-      </c>
-      <c r="T39" t="s">
-        <v>46</v>
-      </c>
-      <c r="V39" t="s">
-        <v>42</v>
-      </c>
-      <c r="W39" t="s">
-        <v>214</v>
-      </c>
-      <c r="X39" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>315</v>
-      </c>
-      <c r="Z39" t="s">
-        <v>325</v>
-      </c>
-      <c r="AA39">
-        <v>2</v>
-      </c>
-      <c r="AB39">
-        <v>2</v>
-      </c>
-      <c r="AC39">
-        <v>2</v>
+      <c r="R39" t="s">
+        <v>84</v>
       </c>
       <c r="AE39" t="s">
-        <v>321</v>
+        <v>349</v>
       </c>
       <c r="AF39">
-        <v>4.3</v>
-      </c>
-      <c r="AG39" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH39" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI39" t="s">
-        <v>140</v>
-      </c>
-      <c r="AJ39" t="s">
-        <v>154</v>
-      </c>
-      <c r="AK39" t="s">
-        <v>134</v>
-      </c>
-      <c r="AL39" t="s">
-        <v>317</v>
-      </c>
-      <c r="AM39" t="s">
-        <v>233</v>
-      </c>
-      <c r="AO39" t="s">
-        <v>319</v>
-      </c>
-      <c r="AP39" t="s">
-        <v>320</v>
-      </c>
-      <c r="AQ39" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR39" t="s">
-        <v>239</v>
-      </c>
-      <c r="AU39" t="s">
-        <v>316</v>
-      </c>
-      <c r="AV39" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW39" t="s">
-        <v>208</v>
-      </c>
-      <c r="AX39" t="s">
-        <v>318</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A40" s="11" t="s">
+      <c r="A40" t="s">
         <v>265</v>
       </c>
       <c r="B40" t="s">
@@ -8820,7 +8813,7 @@
         <v>140</v>
       </c>
       <c r="AJ40" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
       <c r="AK40" t="s">
         <v>134</v>
@@ -8857,41 +8850,41 @@
       </c>
     </row>
     <row r="41" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A41" s="11" t="s">
-        <v>259</v>
+      <c r="A41" t="s">
+        <v>265</v>
       </c>
       <c r="B41" t="s">
         <v>244</v>
       </c>
       <c r="C41" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="D41" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="E41">
         <v>2009</v>
       </c>
       <c r="F41" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="G41">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I41">
-        <v>392</v>
+        <v>472</v>
       </c>
       <c r="J41">
-        <v>401</v>
+        <v>478</v>
       </c>
       <c r="K41" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="M41" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="N41" t="s">
         <v>243</v>
@@ -8903,28 +8896,25 @@
         <v>21</v>
       </c>
       <c r="S41" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="T41" t="s">
         <v>46</v>
       </c>
-      <c r="U41" t="s">
-        <v>58</v>
-      </c>
       <c r="V41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="W41" t="s">
-        <v>58</v>
+        <v>214</v>
       </c>
       <c r="X41" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="Y41" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="Z41" t="s">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="AA41">
         <v>2</v>
@@ -8933,59 +8923,62 @@
         <v>2</v>
       </c>
       <c r="AC41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE41" t="s">
-        <v>311</v>
-      </c>
-      <c r="AF41" s="12">
-        <v>4.5</v>
+        <v>321</v>
+      </c>
+      <c r="AF41">
+        <v>4.3</v>
       </c>
       <c r="AG41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AH41" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="AI41" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="AJ41" t="s">
-        <v>155</v>
+        <v>113</v>
+      </c>
+      <c r="AK41" t="s">
+        <v>134</v>
       </c>
       <c r="AL41" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="AM41" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AO41" t="s">
-        <v>312</v>
+        <v>319</v>
+      </c>
+      <c r="AP41" t="s">
+        <v>320</v>
       </c>
       <c r="AQ41" t="s">
         <v>164</v>
       </c>
       <c r="AR41" t="s">
-        <v>170</v>
-      </c>
-      <c r="AS41" t="s">
-        <v>188</v>
+        <v>239</v>
       </c>
       <c r="AU41" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="AV41" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="AW41" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AX41" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="42" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A42" s="11" t="s">
+      <c r="A42" t="s">
         <v>259</v>
       </c>
       <c r="B42" t="s">
@@ -9066,7 +9059,7 @@
       <c r="AE42" t="s">
         <v>311</v>
       </c>
-      <c r="AF42" s="12">
+      <c r="AF42" s="10">
         <v>4.5</v>
       </c>
       <c r="AG42" t="s">
@@ -9091,7 +9084,7 @@
         <v>312</v>
       </c>
       <c r="AQ42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AR42" t="s">
         <v>170</v>
@@ -9113,41 +9106,41 @@
       </c>
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A43" s="11" t="s">
-        <v>253</v>
+      <c r="A43" t="s">
+        <v>259</v>
       </c>
       <c r="B43" t="s">
         <v>244</v>
       </c>
       <c r="C43" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D43" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="E43">
         <v>2009</v>
       </c>
       <c r="F43" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="G43">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43">
-        <v>41</v>
+        <v>392</v>
       </c>
       <c r="J43">
-        <v>49</v>
+        <v>401</v>
       </c>
       <c r="K43" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="M43" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N43" t="s">
         <v>243</v>
@@ -9158,10 +9151,138 @@
       <c r="Q43" t="s">
         <v>21</v>
       </c>
-      <c r="R43" t="s">
+      <c r="S43" t="s">
+        <v>26</v>
+      </c>
+      <c r="T43" t="s">
+        <v>46</v>
+      </c>
+      <c r="U43" t="s">
+        <v>58</v>
+      </c>
+      <c r="V43" t="s">
+        <v>46</v>
+      </c>
+      <c r="W43" t="s">
+        <v>58</v>
+      </c>
+      <c r="X43" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>308</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>310</v>
+      </c>
+      <c r="AA43">
+        <v>2</v>
+      </c>
+      <c r="AB43">
+        <v>2</v>
+      </c>
+      <c r="AC43">
+        <v>3</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>311</v>
+      </c>
+      <c r="AF43" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH43" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>129</v>
+      </c>
+      <c r="AJ43" t="s">
+        <v>155</v>
+      </c>
+      <c r="AL43" t="s">
+        <v>309</v>
+      </c>
+      <c r="AM43" t="s">
+        <v>231</v>
+      </c>
+      <c r="AO43" t="s">
+        <v>312</v>
+      </c>
+      <c r="AQ43" t="s">
+        <v>165</v>
+      </c>
+      <c r="AR43" t="s">
+        <v>170</v>
+      </c>
+      <c r="AS43" t="s">
+        <v>188</v>
+      </c>
+      <c r="AU43" t="s">
+        <v>313</v>
+      </c>
+      <c r="AV43" t="s">
+        <v>238</v>
+      </c>
+      <c r="AW43" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX43" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="44" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>253</v>
+      </c>
+      <c r="B44" t="s">
+        <v>244</v>
+      </c>
+      <c r="C44" t="s">
+        <v>252</v>
+      </c>
+      <c r="D44" t="s">
+        <v>251</v>
+      </c>
+      <c r="E44">
+        <v>2009</v>
+      </c>
+      <c r="F44" t="s">
+        <v>250</v>
+      </c>
+      <c r="G44">
+        <v>82</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>41</v>
+      </c>
+      <c r="J44">
+        <v>49</v>
+      </c>
+      <c r="K44" t="s">
+        <v>249</v>
+      </c>
+      <c r="M44" t="s">
+        <v>248</v>
+      </c>
+      <c r="N44" t="s">
+        <v>243</v>
+      </c>
+      <c r="O44" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>21</v>
+      </c>
+      <c r="R44" t="s">
         <v>84</v>
       </c>
-      <c r="AF43">
+      <c r="AF44">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -9176,14 +9297,14 @@
     <mergeCell ref="AM1:AP1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="P37:P1048576 Q3:Q36" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="P38:P1048576 Q3:Q37" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH3:AH1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Ecosystem_component</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ3:AQ1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Fishery_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN3:AN1048576 AI3:AJ1048576 AR3:AS1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR3:AS1048576 AI3:AJ1048576 AN3:AN1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>INDIRECT(AH3)</formula1>
     </dataValidation>
   </dataValidations>
@@ -9197,25 +9318,25 @@
           <x14:formula1>
             <xm:f>Validation!$AA$3:$AA$5</xm:f>
           </x14:formula1>
-          <xm:sqref>AA48:AA1048576 AA3:AA46</xm:sqref>
+          <xm:sqref>AA49:AA1048576 AA3:AA47</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>Validation!$AB$3:$AB$5</xm:f>
           </x14:formula1>
-          <xm:sqref>AB48:AB1048576 AB3:AB46</xm:sqref>
+          <xm:sqref>AB49:AB1048576 AB3:AB47</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>Validation!$AC$3:$AC$5</xm:f>
           </x14:formula1>
-          <xm:sqref>AC48:AC1048576 AC3:AC46</xm:sqref>
+          <xm:sqref>AC49:AC1048576 AC3:AC47</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
             <xm:f>'C:\Users\kjova\Downloads\[DataExtractionForm_WP4_Dinesen.xlsx]Validation'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AF43 AF3:AF6</xm:sqref>
+          <xm:sqref>AF44 AF3:AF6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
@@ -9297,7 +9418,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AY38"/>
+  <dimension ref="A1:AX38"/>
   <sheetViews>
     <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
@@ -9314,70 +9435,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="18" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="16" t="s">
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="17" t="s">
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="17"/>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="17"/>
-      <c r="AM1" s="10" t="s">
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="13" t="s">
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="9" t="s">
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AV1" s="9"/>
-      <c r="AW1" s="9"/>
-      <c r="AX1" s="9"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
     </row>
     <row r="2" spans="1:50" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -9699,7 +9820,7 @@
       <c r="AW5" t="s">
         <v>210</v>
       </c>
-      <c r="AX5" s="8"/>
+      <c r="AX5" s="7"/>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="R6" t="s">
@@ -10087,7 +10208,7 @@
       </c>
     </row>
     <row r="19" spans="34:48" x14ac:dyDescent="0.35">
-      <c r="AQ19" s="7" t="s">
+      <c r="AQ19" t="s">
         <v>113</v>
       </c>
     </row>
@@ -10290,7 +10411,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="33" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AH33" t="s">
         <v>155</v>
       </c>
@@ -10310,7 +10431,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="34" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AI34" t="s">
         <v>157</v>
       </c>
@@ -10323,9 +10444,8 @@
       <c r="AV34" t="s">
         <v>194</v>
       </c>
-      <c r="AY34" s="7"/>
     </row>
-    <row r="35" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="35" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AI35" t="s">
         <v>113</v>
       </c>
@@ -10339,7 +10459,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="36" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="36" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AU36" t="s">
         <v>211</v>
       </c>
@@ -10347,10 +10467,10 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="37" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AL37" s="5"/>
     </row>
-    <row r="38" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="38" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AL38" s="6"/>
       <c r="AM38" s="6"/>
       <c r="AN38" s="6"/>
@@ -10410,51 +10530,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="17" t="s">
+      <c r="P1" s="14"/>
+      <c r="Q1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="10" t="s">
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="13" t="s">
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="14" t="s">
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
     </row>
     <row r="2" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -10977,7 +11097,7 @@
       <c r="G12" t="s">
         <v>76</v>
       </c>
-      <c r="Q12" s="7" t="s">
+      <c r="Q12" t="s">
         <v>221</v>
       </c>
       <c r="R12" t="s">
@@ -11298,6 +11418,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="125e2131eddd38cce17ebc9527d7a9d7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="553f2d8843fd2aa64b81f9e8c63a6619">
     <xsd:element name="properties">
@@ -11411,22 +11546,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5119AE1-18E6-4AE7-B94D-A5692B077F3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11440,21 +11583,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>